<commit_message>
get histogram excel sheet
</commit_message>
<xml_diff>
--- a/Get Histogram Observations (10MB file).xlsx
+++ b/Get Histogram Observations (10MB file).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SSD" sheetId="1" r:id="rId1"/>
@@ -486,6 +486,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1416</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7489</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5518</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7489</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6553</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9532</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5242</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4369</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -997,7 +1027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1134,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="B2:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1155,71 +1185,111 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="1">
+        <v>1416</v>
+      </c>
+      <c r="C2" s="1">
+        <v>74</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="1">
+        <v>4993</v>
+      </c>
+      <c r="C3" s="1">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="1">
+        <v>7489</v>
+      </c>
+      <c r="C4" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="1">
+        <v>5518</v>
+      </c>
+      <c r="C5" s="1">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="1">
+        <v>5242</v>
+      </c>
+      <c r="C6" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="1">
+        <v>7489</v>
+      </c>
+      <c r="C7" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="1">
+        <v>6553</v>
+      </c>
+      <c r="C8" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="1">
+        <v>9532</v>
+      </c>
+      <c r="C9" s="1">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="1">
+        <v>5242</v>
+      </c>
+      <c r="C10" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1">
+        <v>4369</v>
+      </c>
+      <c r="C11" s="1">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>